<commit_message>
Solver rdy but need to check it
Na ten moment odpalając maina rozwiązuje przykład ze skryptu.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wutwaw-my.sharepoint.com/personal/01142312_pw_edu_pl/Documents/PW/Semy/Sem6/DUW - Dynamika Układów Wieloczłonowych/1. Zadanie domowe - Matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="11_AD4DADEC636C813AC809E43EA81C70E85BDEDD89" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0D51EF12-E87B-43F7-A56B-64DB7FE27B7E}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="11_AD4DADEC636C813AC809E43EA81C70E85BDEDD89" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5B55B224-012C-4FE2-8FE2-9E48E22402D3}"/>
   <bookViews>
     <workbookView xWindow="12285" yWindow="570" windowWidth="14700" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
     <t>Równania więzów kierujących (jeśli pusty to nie ma więzu)</t>
   </si>
   <si>
-    <t>2*sin(t^2)</t>
+    <t>t^2+pi/2</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +526,9 @@
       <c r="D2">
         <v>1</v>
       </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -576,9 +579,6 @@
       </c>
       <c r="G5">
         <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>